<commit_message>
WebEventListener added. ExtentReport added. Right approch to data driven testing used.
</commit_message>
<xml_diff>
--- a/IStafz v1.0/testdata/Book1.xlsx
+++ b/IStafz v1.0/testdata/Book1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="11340" windowHeight="2970"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13575" windowHeight="2145" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
@@ -12,19 +12,13 @@
     <sheet name="BuildNumber" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A2:K9"/>
+  <oleSize ref="A1:J7"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
-    <t>USERNAME</t>
-  </si>
-  <si>
-    <t>PASSWORD</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -34,19 +28,25 @@
     <t>manager1</t>
   </si>
   <si>
+    <t>abcd123</t>
+  </si>
+  <si>
+    <t>123abc</t>
+  </si>
+  <si>
+    <t>(build 1032_35)</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>buildnumber</t>
+  </si>
+  <si>
     <t>admin1</t>
-  </si>
-  <si>
-    <t>abcd123</t>
-  </si>
-  <si>
-    <t>123abc</t>
-  </si>
-  <si>
-    <t>BUILDNUMBER</t>
-  </si>
-  <si>
-    <t>(build 1032_35)</t>
   </si>
 </sst>
 </file>
@@ -387,26 +387,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="115" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -418,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -430,34 +430,34 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -469,18 +469,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="115" workbookViewId="0">
+      <selection activeCell="E5" sqref="E4:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>8</v>
@@ -488,13 +488,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>